<commit_message>
added data and newest main from rbpi
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="24">
   <si>
     <t xml:space="preserve">Baseline 1</t>
   </si>
@@ -1376,12 +1376,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.51"/>
   </cols>
@@ -2512,13 +2512,13 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.99"/>
@@ -3258,16 +3258,25 @@
       <c r="A37" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="9"/>
+      <c r="B37" s="9" t="n">
+        <v>199</v>
+      </c>
+      <c r="C37" s="9" t="n">
+        <v>40</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <f aca="false">1-C37/B37</f>
+        <v>0.798994974874372</v>
+      </c>
+      <c r="E37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9" t="n">
+        <v>-89.51</v>
+      </c>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -3276,16 +3285,25 @@
       <c r="A38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="9"/>
+      <c r="B38" s="9" t="n">
+        <v>199</v>
+      </c>
+      <c r="C38" s="9" t="n">
+        <v>46</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <f aca="false">1-C38/B38</f>
+        <v>0.768844221105528</v>
+      </c>
+      <c r="E38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9" t="n">
+        <v>-91.59</v>
+      </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
@@ -3294,16 +3312,25 @@
       <c r="A39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="9"/>
+      <c r="B39" s="9" t="n">
+        <v>199</v>
+      </c>
+      <c r="C39" s="9" t="n">
+        <v>22</v>
+      </c>
+      <c r="D39" s="10" t="n">
+        <f aca="false">1-C39/B39</f>
+        <v>0.889447236180904</v>
+      </c>
+      <c r="E39" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9" t="n">
+        <v>-90.81</v>
+      </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
@@ -3354,12 +3381,15 @@
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>14</v>
+      <c r="D42" s="10" t="e">
+        <f aca="false">1-C42/B42</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E42" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="7"/>
@@ -3372,12 +3402,15 @@
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>14</v>
+      <c r="D43" s="10" t="e">
+        <f aca="false">1-C43/B43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E43" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="7"/>
@@ -3390,12 +3423,15 @@
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>14</v>
+      <c r="D44" s="10" t="e">
+        <f aca="false">1-C44/B44</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E44" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="7"/>
@@ -3437,12 +3473,15 @@
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>14</v>
+      <c r="D47" s="10" t="e">
+        <f aca="false">1-C47/B47</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="7"/>
@@ -3455,12 +3494,15 @@
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>14</v>
+      <c r="D48" s="10" t="e">
+        <f aca="false">1-C48/B48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E48" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G48" s="9"/>
       <c r="H48" s="7"/>
@@ -3473,12 +3515,15 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>14</v>
+      <c r="D49" s="10" t="e">
+        <f aca="false">1-C49/B49</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E49" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="9" t="n">
+        <v>0</v>
       </c>
       <c r="G49" s="9"/>
       <c r="H49" s="7"/>
@@ -3529,29 +3574,29 @@
       <c r="A52" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="9" t="e">
+      <c r="B52" s="9" t="n">
         <f aca="false">AVERAGE(B32,B37,B47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C52" s="9" t="e">
+        <v>199</v>
+      </c>
+      <c r="C52" s="9" t="n">
         <f aca="false">AVERAGE(C32,C37,C47)</f>
-        <v>#DIV/0!</v>
+        <v>40</v>
       </c>
       <c r="D52" s="9" t="e">
         <f aca="false">AVERAGE(D32,D37,D47)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E52" s="9" t="e">
+      <c r="E52" s="9" t="n">
         <f aca="false">AVERAGE(E32,E37,E47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F52" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="F52" s="9" t="n">
         <f aca="false">AVERAGE(F32,F37,F47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G52" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="G52" s="9" t="n">
         <f aca="false">AVERAGE(G32,G37,G47)</f>
-        <v>#DIV/0!</v>
+        <v>-89.51</v>
       </c>
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
@@ -3561,29 +3606,29 @@
       <c r="A53" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B53" s="9" t="e">
+      <c r="B53" s="9" t="n">
         <f aca="false">AVERAGE(B33,B38,B48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C53" s="9" t="e">
+        <v>199</v>
+      </c>
+      <c r="C53" s="9" t="n">
         <f aca="false">AVERAGE(C33,C38,C48)</f>
-        <v>#DIV/0!</v>
+        <v>46</v>
       </c>
       <c r="D53" s="9" t="e">
         <f aca="false">AVERAGE(D33,D38,D48)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E53" s="9" t="e">
+      <c r="E53" s="9" t="n">
         <f aca="false">AVERAGE(E33,E38,E48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F53" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="F53" s="9" t="n">
         <f aca="false">AVERAGE(F33,F38,F48)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G53" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="G53" s="9" t="n">
         <f aca="false">AVERAGE(G33,G38,G48)</f>
-        <v>#DIV/0!</v>
+        <v>-91.59</v>
       </c>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
@@ -3593,29 +3638,29 @@
       <c r="A54" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="9" t="e">
+      <c r="B54" s="9" t="n">
         <f aca="false">AVERAGE(B34,B39,B49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C54" s="9" t="e">
+        <v>199</v>
+      </c>
+      <c r="C54" s="9" t="n">
         <f aca="false">AVERAGE(C34,C39,C49)</f>
-        <v>#DIV/0!</v>
+        <v>22</v>
       </c>
       <c r="D54" s="9" t="e">
         <f aca="false">AVERAGE(D34,D39,D49)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E54" s="9" t="e">
+      <c r="E54" s="9" t="n">
         <f aca="false">AVERAGE(E34,E39,E49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F54" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="F54" s="9" t="n">
         <f aca="false">AVERAGE(F34,F39,F49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G54" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="G54" s="9" t="n">
         <f aca="false">AVERAGE(G34,G39,G49)</f>
-        <v>#DIV/0!</v>
+        <v>-90.81</v>
       </c>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>

</xml_diff>

<commit_message>
added newest data baseline 1_2
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -372,17 +372,17 @@
   <dimension ref="A1:J181"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.43"/>
   </cols>
   <sheetData>
@@ -624,7 +624,9 @@
       <c r="B13" s="9" t="n">
         <v>100</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="9" t="n">
+        <v>0</v>
+      </c>
       <c r="D13" s="10" t="n">
         <f aca="false">1-C13/B13</f>
         <v>1</v>
@@ -635,7 +637,9 @@
       <c r="F13" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="9" t="n">
+        <v>-92.86</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -647,7 +651,9 @@
       <c r="B14" s="9" t="n">
         <v>100</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="9" t="n">
+        <v>0</v>
+      </c>
       <c r="D14" s="10" t="n">
         <f aca="false">1-C14/B14</f>
         <v>1</v>
@@ -658,7 +664,9 @@
       <c r="F14" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="9" t="n">
+        <v>-93.64</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -670,7 +678,9 @@
       <c r="B15" s="9" t="n">
         <v>100</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="9" t="n">
+        <v>0</v>
+      </c>
       <c r="D15" s="10" t="n">
         <f aca="false">1-C15/B15</f>
         <v>1</v>
@@ -681,7 +691,9 @@
       <c r="F15" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="9" t="n">
+        <v>-94.18</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -861,7 +873,7 @@
       </c>
       <c r="G23" s="9" t="n">
         <f aca="false">AVERAGE(G8,G13,G18)</f>
-        <v>-92.84</v>
+        <v>-92.85</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -893,7 +905,7 @@
       </c>
       <c r="G24" s="9" t="n">
         <f aca="false">AVERAGE(G9,G14,G19)</f>
-        <v>-93.41</v>
+        <v>-93.525</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -925,7 +937,7 @@
       </c>
       <c r="G25" s="9" t="n">
         <f aca="false">AVERAGE(G10,G15,G20)</f>
-        <v>-92.94</v>
+        <v>-93.56</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -5022,7 +5034,7 @@
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>

</xml_diff>

<commit_message>
added newest data. data complete
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -399,11 +399,11 @@
   </sheetPr>
   <dimension ref="A1:X182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J99" activeCellId="0" sqref="J99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P176" activeCellId="0" sqref="P176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -4364,32 +4364,32 @@
         <v>100</v>
       </c>
       <c r="C122" s="9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D122" s="10" t="n">
         <f aca="false">1-C122/B122</f>
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="E122" s="9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F122" s="9" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="G122" s="9" t="n">
         <f aca="false">F122+E122</f>
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="H122" s="9" t="n">
         <f aca="false">G122/B122</f>
-        <v>1.18</v>
+        <v>0.85</v>
       </c>
       <c r="I122" s="9" t="n">
         <f aca="false">1-(C122+E122)/B122</f>
-        <v>0.98</v>
+        <v>0.85</v>
       </c>
       <c r="J122" s="9" t="n">
-        <v>-100.63</v>
+        <v>-96.7</v>
       </c>
       <c r="K122" s="7"/>
       <c r="L122" s="7"/>
@@ -4403,32 +4403,32 @@
         <v>100</v>
       </c>
       <c r="C123" s="9" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D123" s="10" t="n">
         <f aca="false">1-C123/B123</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E123" s="9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F123" s="9" t="n">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="G123" s="9" t="n">
         <f aca="false">F123+E123</f>
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="H123" s="9" t="n">
         <f aca="false">G123/B123</f>
-        <v>1.18</v>
+        <v>0.75</v>
       </c>
       <c r="I123" s="9" t="n">
         <f aca="false">1-(C123+E123)/B123</f>
-        <v>0.98</v>
+        <v>0.75</v>
       </c>
       <c r="J123" s="9" t="n">
-        <v>-97.56</v>
+        <v>-96.87</v>
       </c>
       <c r="K123" s="7"/>
       <c r="L123" s="7"/>
@@ -4442,32 +4442,32 @@
         <v>100</v>
       </c>
       <c r="C124" s="9" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D124" s="10" t="n">
         <f aca="false">1-C124/B124</f>
-        <v>1</v>
+        <v>0.54</v>
       </c>
       <c r="E124" s="9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F124" s="9" t="n">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="G124" s="9" t="n">
         <f aca="false">F124+E124</f>
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="H124" s="9" t="n">
         <f aca="false">G124/B124</f>
-        <v>1.15</v>
+        <v>0.54</v>
       </c>
       <c r="I124" s="9" t="n">
         <f aca="false">1-(C124+E124)/B124</f>
-        <v>0.98</v>
+        <v>0.54</v>
       </c>
       <c r="J124" s="9" t="n">
-        <v>-98.75</v>
+        <v>-101.54</v>
       </c>
       <c r="K124" s="7"/>
       <c r="L124" s="7"/>
@@ -4532,35 +4532,35 @@
       </c>
       <c r="C127" s="9" t="n">
         <f aca="false">AVERAGE(C112,C117,C122)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D127" s="12" t="n">
         <f aca="false">1-C127/B127</f>
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="E127" s="12" t="n">
         <f aca="false">AVERAGE(E112,E117,E122)</f>
-        <v>8.33333333333333</v>
+        <v>7.66666666666667</v>
       </c>
       <c r="F127" s="12" t="n">
         <f aca="false">AVERAGE(F112,F117,F122)</f>
-        <v>109</v>
+        <v>98.6666666666667</v>
       </c>
       <c r="G127" s="12" t="n">
         <f aca="false">F127+E127</f>
-        <v>117.333333333333</v>
+        <v>106.333333333333</v>
       </c>
       <c r="H127" s="12" t="n">
         <f aca="false">G127/B127</f>
-        <v>1.17333333333333</v>
+        <v>1.06333333333333</v>
       </c>
       <c r="I127" s="12" t="n">
         <f aca="false">1-(C127+E127)/B127</f>
-        <v>0.916666666666667</v>
+        <v>0.873333333333333</v>
       </c>
       <c r="J127" s="9" t="n">
         <f aca="false">AVERAGE(J112,J117,J122)</f>
-        <v>-102.736666666667</v>
+        <v>-101.426666666667</v>
       </c>
       <c r="K127" s="11"/>
       <c r="L127" s="11"/>
@@ -4576,35 +4576,35 @@
       </c>
       <c r="C128" s="9" t="n">
         <f aca="false">AVERAGE(C113,C118,C123)</f>
-        <v>0</v>
+        <v>8.33333333333333</v>
       </c>
       <c r="D128" s="12" t="n">
         <f aca="false">1-C128/B128</f>
-        <v>1</v>
+        <v>0.916666666666667</v>
       </c>
       <c r="E128" s="12" t="n">
         <f aca="false">AVERAGE(E113,E118,E123)</f>
-        <v>3.33333333333333</v>
+        <v>2.66666666666667</v>
       </c>
       <c r="F128" s="12" t="n">
         <f aca="false">AVERAGE(F113,F118,F123)</f>
-        <v>112.666666666667</v>
+        <v>99</v>
       </c>
       <c r="G128" s="12" t="n">
         <f aca="false">F128+E128</f>
-        <v>116</v>
+        <v>101.666666666667</v>
       </c>
       <c r="H128" s="12" t="n">
         <f aca="false">G128/B128</f>
-        <v>1.16</v>
+        <v>1.01666666666667</v>
       </c>
       <c r="I128" s="12" t="n">
         <f aca="false">1-(C128+E128)/B128</f>
-        <v>0.966666666666667</v>
+        <v>0.89</v>
       </c>
       <c r="J128" s="9" t="n">
         <f aca="false">AVERAGE(J113,J118,J123)</f>
-        <v>-102.32</v>
+        <v>-102.09</v>
       </c>
       <c r="K128" s="11"/>
       <c r="L128" s="11"/>
@@ -4620,35 +4620,35 @@
       </c>
       <c r="C129" s="9" t="n">
         <f aca="false">AVERAGE(C114,C119,C124)</f>
-        <v>0</v>
+        <v>15.3333333333333</v>
       </c>
       <c r="D129" s="12" t="n">
         <f aca="false">1-C129/B129</f>
-        <v>1</v>
+        <v>0.846666666666667</v>
       </c>
       <c r="E129" s="12" t="n">
         <f aca="false">AVERAGE(E114,E119,E124)</f>
-        <v>3.33333333333333</v>
+        <v>2.66666666666667</v>
       </c>
       <c r="F129" s="12" t="n">
         <f aca="false">AVERAGE(F114,F119,F124)</f>
-        <v>116</v>
+        <v>96.3333333333333</v>
       </c>
       <c r="G129" s="12" t="n">
         <f aca="false">F129+E129</f>
-        <v>119.333333333333</v>
+        <v>99</v>
       </c>
       <c r="H129" s="12" t="n">
         <f aca="false">G129/B129</f>
-        <v>1.19333333333333</v>
+        <v>0.99</v>
       </c>
       <c r="I129" s="12" t="n">
         <f aca="false">1-(C129+E129)/B129</f>
-        <v>0.966666666666667</v>
+        <v>0.82</v>
       </c>
       <c r="J129" s="9" t="n">
         <f aca="false">AVERAGE(J114,J119,J124)</f>
-        <v>-101.866666666667</v>
+        <v>-102.796666666667</v>
       </c>
       <c r="K129" s="11"/>
       <c r="L129" s="11"/>
@@ -7235,7 +7235,7 @@
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>

</xml_diff>

<commit_message>
added visualisation for data
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -235,7 +235,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -301,11 +301,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -381,7 +376,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -458,11 +453,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,7 +541,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -550,10 +553,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501125952432366"/>
-          <c:y val="0.101047493693101"/>
-          <c:w val="0.90066940185705"/>
-          <c:h val="0.746791707798618"/>
+          <c:x val="0.0501227133567796"/>
+          <c:y val="0.101034637876743"/>
+          <c:w val="0.90061483187005"/>
+          <c:h val="0.746693657219973"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -564,7 +567,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$O$102:$O$102</c:f>
+              <c:f>Baseline_100pkt!$O$69:$O$69</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -574,7 +577,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -600,6 +605,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -610,10 +616,11 @@
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln>
+              <a:ln w="12600">
                 <a:solidFill>
                   <a:srgbClr val="f10d0c"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
@@ -629,7 +636,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Baseline_100pkt!$R$102:$R$104</c:f>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -647,7 +654,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Baseline_100pkt!$R$102:$R$104</c:f>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -673,7 +680,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Baseline_100pkt!$Q$102:$Q$104</c:f>
+              <c:f>Baseline_100pkt!$Q$69:$Q$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -691,7 +698,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Baseline_100pkt!$P$102:$P$104</c:f>
+              <c:f>Baseline_100pkt!$P$69:$P$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -714,7 +721,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$O$106:$O$106</c:f>
+              <c:f>Baseline_100pkt!$O$73:$O$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -724,7 +731,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -750,6 +759,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -760,10 +770,11 @@
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln>
+              <a:ln w="12600">
                 <a:solidFill>
                   <a:srgbClr val="069a2e"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
@@ -779,7 +790,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Baseline_100pkt!$R$106:$R$108</c:f>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -797,7 +808,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Baseline_100pkt!$R$106:$R$108</c:f>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -823,7 +834,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Baseline_100pkt!$Q$106:$Q$108</c:f>
+              <c:f>Baseline_100pkt!$Q$73:$Q$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -841,7 +852,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Baseline_100pkt!$P$106:$P$108</c:f>
+              <c:f>Baseline_100pkt!$P$73:$P$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -859,14 +870,14 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44127482"/>
-        <c:axId val="36877102"/>
+        <c:axId val="51573984"/>
+        <c:axId val="13816737"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44127482"/>
+        <c:axId val="51573984"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
-          <c:max val="31"/>
+          <c:max val="35"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -908,7 +919,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -925,20 +936,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36877102"/>
+        <c:crossAx val="13816737"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36877102"/>
+        <c:axId val="13816737"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -992,7 +1003,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1008,13 +1019,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44127482"/>
+        <c:crossAx val="51573984"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -1057,7 +1068,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1068,16 +1079,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>633960</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>245880</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>54000</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>183600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1641600</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1820160</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1085,8 +1096,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="18402840" y="16101720"/>
-        <a:ext cx="11670120" cy="6564240"/>
+        <a:off x="18637200" y="18231480"/>
+        <a:ext cx="14227920" cy="8002440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1106,15 +1117,15 @@
   </sheetPr>
   <dimension ref="A1:AP182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L67" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U88" activeCellId="0" sqref="U88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L77" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R121" activeCellId="0" sqref="R121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.41"/>
@@ -1129,7 +1140,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="32.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="33.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="36.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="36.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="44.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="25.68"/>
@@ -1137,7 +1148,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="13.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="25.68"/>
@@ -6081,9 +6092,21 @@
       <c r="L67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="D68" s="4"/>
+      <c r="O68" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="P68" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q68" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R68" s="18" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
@@ -6121,6 +6144,21 @@
       </c>
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
+      <c r="O69" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P69" s="21" t="n">
+        <f aca="false">R58</f>
+        <v>0.62</v>
+      </c>
+      <c r="Q69" s="18" t="n">
+        <f aca="false">T58</f>
+        <v>30</v>
+      </c>
+      <c r="R69" s="21" t="n">
+        <f aca="false">S58</f>
+        <v>0.117015351952607</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
@@ -6160,6 +6198,19 @@
       <c r="K70" s="7"/>
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="21" t="n">
+        <f aca="false">R61</f>
+        <v>0.72</v>
+      </c>
+      <c r="Q70" s="18" t="n">
+        <f aca="false">T61</f>
+        <v>15</v>
+      </c>
+      <c r="R70" s="21" t="n">
+        <f aca="false">S61</f>
+        <v>0.130398250385899</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
@@ -6199,6 +6250,19 @@
       <c r="K71" s="7"/>
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
+      <c r="O71" s="18"/>
+      <c r="P71" s="21" t="n">
+        <f aca="false">R64</f>
+        <v>0.54</v>
+      </c>
+      <c r="Q71" s="18" t="n">
+        <f aca="false">T64</f>
+        <v>5</v>
+      </c>
+      <c r="R71" s="21" t="n">
+        <f aca="false">S64</f>
+        <v>0.0945946517946345</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
@@ -6238,8 +6302,12 @@
       <c r="K72" s="7"/>
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O72" s="22"/>
+      <c r="P72" s="22"/>
+      <c r="Q72" s="22"/>
+      <c r="R72" s="22"/>
+    </row>
+    <row r="73" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -6250,6 +6318,21 @@
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
+      <c r="O73" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="P73" s="21" t="n">
+        <f aca="false">X58</f>
+        <v>0.962222222222222</v>
+      </c>
+      <c r="Q73" s="18" t="n">
+        <f aca="false">T58</f>
+        <v>30</v>
+      </c>
+      <c r="R73" s="21" t="n">
+        <f aca="false">Y58</f>
+        <v>0.013471506281091</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
@@ -6287,6 +6370,19 @@
       </c>
       <c r="L74" s="11"/>
       <c r="M74" s="11"/>
+      <c r="O74" s="18"/>
+      <c r="P74" s="21" t="n">
+        <f aca="false">X61</f>
+        <v>0.95</v>
+      </c>
+      <c r="Q74" s="18" t="n">
+        <f aca="false">T61</f>
+        <v>15</v>
+      </c>
+      <c r="R74" s="21" t="n">
+        <f aca="false">Y61</f>
+        <v>0.0288675134594813</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
@@ -6331,6 +6427,19 @@
       <c r="K75" s="11"/>
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
+      <c r="O75" s="18"/>
+      <c r="P75" s="21" t="n">
+        <f aca="false">X64</f>
+        <v>0.61</v>
+      </c>
+      <c r="Q75" s="18" t="n">
+        <f aca="false">T64</f>
+        <v>5</v>
+      </c>
+      <c r="R75" s="21" t="n">
+        <f aca="false">Y64</f>
+        <v>0.0835330939076111</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
@@ -6443,120 +6552,14 @@
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O101" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="P101" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q101" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="R101" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O102" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P102" s="20" t="n">
-        <f aca="false">R58</f>
-        <v>0.62</v>
-      </c>
-      <c r="Q102" s="18" t="n">
-        <f aca="false">T58</f>
-        <v>30</v>
-      </c>
-      <c r="R102" s="20" t="n">
-        <f aca="false">S58</f>
-        <v>0.117015351952607</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O103" s="18"/>
-      <c r="P103" s="20" t="n">
-        <f aca="false">R61</f>
-        <v>0.72</v>
-      </c>
-      <c r="Q103" s="18" t="n">
-        <f aca="false">T61</f>
-        <v>15</v>
-      </c>
-      <c r="R103" s="20" t="n">
-        <f aca="false">S61</f>
-        <v>0.130398250385899</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O104" s="18"/>
-      <c r="P104" s="20" t="n">
-        <f aca="false">R64</f>
-        <v>0.54</v>
-      </c>
-      <c r="Q104" s="18" t="n">
-        <f aca="false">T64</f>
-        <v>5</v>
-      </c>
-      <c r="R104" s="20" t="n">
-        <f aca="false">S64</f>
-        <v>0.0945946517946345</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O105" s="18"/>
-      <c r="P105" s="18"/>
-      <c r="Q105" s="18"/>
-      <c r="R105" s="18"/>
-    </row>
-    <row r="106" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O106" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="P106" s="20" t="n">
-        <f aca="false">X58</f>
-        <v>0.962222222222222</v>
-      </c>
-      <c r="Q106" s="18" t="n">
-        <f aca="false">T58</f>
-        <v>30</v>
-      </c>
-      <c r="R106" s="20" t="n">
-        <f aca="false">Y58</f>
-        <v>0.013471506281091</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O107" s="18"/>
-      <c r="P107" s="20" t="n">
-        <f aca="false">X61</f>
-        <v>0.95</v>
-      </c>
-      <c r="Q107" s="18" t="n">
-        <f aca="false">T61</f>
-        <v>15</v>
-      </c>
-      <c r="R107" s="20" t="n">
-        <f aca="false">Y61</f>
-        <v>0.0288675134594813</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O108" s="18"/>
-      <c r="P108" s="20" t="n">
-        <f aca="false">X64</f>
-        <v>0.61</v>
-      </c>
-      <c r="Q108" s="18" t="n">
-        <f aca="false">T64</f>
-        <v>5</v>
-      </c>
-      <c r="R108" s="20" t="n">
-        <f aca="false">Y64</f>
-        <v>0.0835330939076111</v>
-      </c>
-    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7741,7 +7744,7 @@
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>

</xml_diff>

<commit_message>
added new data vis
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -528,7 +528,7 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF069A2E"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF729FCF"/>
@@ -560,11 +560,11 @@
       <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF069A2E"/>
+      <rgbColor rgb="FF3FAF46"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
@@ -576,7 +576,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -588,10 +588,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501277866342772"/>
-          <c:y val="0.101043728630556"/>
-          <c:w val="0.900554163819935"/>
-          <c:h val="0.746670865574951"/>
+          <c:x val="0.0501290551141252"/>
+          <c:y val="0.101048274620957"/>
+          <c:w val="0.900526342426236"/>
+          <c:h val="0.746659468214334"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -905,11 +905,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48607275"/>
-        <c:axId val="77110964"/>
+        <c:axId val="63716207"/>
+        <c:axId val="16977"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48607275"/>
+        <c:axId val="63716207"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -977,14 +977,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77110964"/>
+        <c:crossAx val="16977"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77110964"/>
+        <c:axId val="16977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1060,7 +1060,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48607275"/>
+        <c:crossAx val="63716207"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -1110,7 +1110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1177,6 +1177,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1195,6 +1196,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1347,6 +1349,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1513,6 +1516,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1531,6 +1535,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1683,6 +1688,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1835,6 +1841,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2001,6 +2008,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2019,6 +2027,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2128,11 +2137,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="12847412"/>
-        <c:axId val="89591949"/>
+        <c:axId val="49806575"/>
+        <c:axId val="55424121"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12847412"/>
+        <c:axId val="49806575"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -2177,7 +2186,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2199,13 +2208,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89591949"/>
+        <c:crossAx val="55424121"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89591949"/>
+        <c:axId val="55424121"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -2259,7 +2268,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2281,10 +2290,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12847412"/>
+        <c:crossAx val="49806575"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.1"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2323,7 +2332,1680 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$82</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff6d6d"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff6d6d"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff6d6d"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="square"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="ff6d6d"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$82:$Q$84</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0435889894354067</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0152752523165195</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.155670592384475</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$82:$Q$84</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0435889894354067</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0152752523165195</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.155670592384475</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ff6d6d"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$82:$R$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$82:$P$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.863333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.623333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$86:$Q$88</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0152752523165195</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.161658075373095</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.225018517756502</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$86:$Q$88</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0152752523165195</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.161658075373095</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.225018517756502</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="f10d0c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$86:$R$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$86:$P$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.486666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.616666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.436666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$90</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff3838"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff3838"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff3838"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="ff3838"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$90:$Q$92</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0503322295684717</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.030550504633039</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0585946527708232</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$90:$Q$92</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0503322295684717</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.030550504633039</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0585946527708232</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="ff3838"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$90:$R$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$90:$P$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.676666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.556666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$95</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$95:$Q$97</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0173205080756888</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0568624070307733</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.300887575903913</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$95:$Q$97</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0173205080756888</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0568624070307733</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.300887575903913</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="069a2e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$95:$R$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$95:$P$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.916666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.616666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$99</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3faf46"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="3faf46"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3faf46"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$99:$Q$101</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.023094010767585</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.221434715736565</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$99:$Q$101</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.023094010767585</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.221434715736565</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="3faf46"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$99:$R$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$99:$P$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.966666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.523333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$N$103</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="77bc65"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="77bc65"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="77bc65"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="77bc65"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$103:$Q$105</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0378593889720018</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0152752523165194</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$Q$103:$Q$105</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0378593889720018</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0152752523165194</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.02</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="77bc65"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$103:$R$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$103:$P$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.946666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.966666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="15831808"/>
+        <c:axId val="90436232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="15831808"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="35"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>sending interval in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90436232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90436232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>package delivery ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15831808"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0501290551141252"/>
+          <c:y val="0.101048274620957"/>
+          <c:w val="0.900526342426236"/>
+          <c:h val="0.746659468214334"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$O$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw LoRa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.117015351952607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.130398250385899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0945946517946345</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.117015351952607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.130398250385899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0945946517946345</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="f10d0c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$Q$69:$Q$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$69:$P$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$O$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAC Layer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.013471506281091</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0835330939076111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.013471506281091</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0835330939076111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="069a2e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$Q$73:$Q$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$73:$P$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.962222222222222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="47505677"/>
+        <c:axId val="31888316"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="47505677"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="35"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>sending interval in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:solidFill>
+              <a:srgbClr val="cccccc"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31888316"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="31888316"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>package delivery ratio (PDR)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47505677"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.05"/>
+        <c:minorUnit val="0.025"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -2341,9 +4023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>214560</xdr:rowOff>
+      <xdr:rowOff>214200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2351,8 +4033,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33293880" y="16205400"/>
-        <a:ext cx="14226480" cy="8001720"/>
+        <a:off x="33294600" y="16205400"/>
+        <a:ext cx="14226120" cy="8001360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2371,9 +4053,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1874160</xdr:colOff>
+      <xdr:colOff>1873800</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2382,11 +4064,71 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17734680" y="25659360"/>
-        <a:ext cx="14334840" cy="8062920"/>
+        <a:ext cx="14335200" cy="8062560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>794160</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>169560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1890720</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>116640</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="17751600" y="34045200"/>
+        <a:ext cx="14335200" cy="8021880"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>2609280</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>5040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>611280</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>147600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="32805360" y="24498000"/>
+        <a:ext cx="14226120" cy="8001360"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2402,11 +4144,11 @@
   </sheetPr>
   <dimension ref="A1:AP182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N102" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T103" activeCellId="0" sqref="T103"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P96" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U170" activeCellId="0" sqref="U170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
@@ -2419,7 +4161,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="41.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="41.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="32.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="26.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.63"/>
@@ -8428,7 +10170,7 @@
   </sheetPr>
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -9450,11 +11192,11 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>

</xml_diff>

<commit_message>
created and updated figures
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="86">
   <si>
     <t xml:space="preserve">Baseline 1</t>
   </si>
@@ -129,6 +129,12 @@
     <t xml:space="preserve">Backoff + Retransmission </t>
   </si>
   <si>
+    <t xml:space="preserve">Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redundancy experiment PDRs</t>
+  </si>
+  <si>
     <t xml:space="preserve">30s Raw LoRa</t>
   </si>
   <si>
@@ -141,16 +147,25 @@
     <t xml:space="preserve">Exp 30 Backoff + Retransmission #1 </t>
   </si>
   <si>
+    <t xml:space="preserve">no fault</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exp 30 Raw Lora #2</t>
   </si>
   <si>
     <t xml:space="preserve">Exp 30 Backoff + Retransmission #2</t>
   </si>
   <si>
+    <t xml:space="preserve">fault</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exp 30 Raw Lora #3</t>
   </si>
   <si>
     <t xml:space="preserve">Exp 30 Backoff + Retransmission #3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redundant</t>
   </si>
   <si>
     <t xml:space="preserve">15s Raw LoRa</t>
@@ -225,9 +240,6 @@
     <t xml:space="preserve">Median perf. Incr. Sigma</t>
   </si>
   <si>
-    <t xml:space="preserve">Board</t>
-  </si>
-  <si>
     <t xml:space="preserve">Experiment</t>
   </si>
   <si>
@@ -238,6 +250,24 @@
   </si>
   <si>
     <t xml:space="preserve">3 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 1 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 2 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board 3 MAC</t>
   </si>
   <si>
     <t xml:space="preserve">(3 boards, 15 min)</t>
@@ -262,7 +292,7 @@
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -329,6 +359,11 @@
     </font>
     <font>
       <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -527,8 +562,8 @@
       <rgbColor rgb="FF127622"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF069A2E"/>
+      <rgbColor rgb="FFA7074B"/>
+      <rgbColor rgb="FF168253"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF729FCF"/>
@@ -560,11 +595,11 @@
       <rgbColor rgb="FF77BC65"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF3838"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF3FAF46"/>
+      <rgbColor rgb="FF069A2E"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
@@ -588,10 +623,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501290551141252"/>
-          <c:y val="0.101048274620957"/>
-          <c:w val="0.900526342426236"/>
-          <c:h val="0.746659468214334"/>
+          <c:x val="0.0501315922664237"/>
+          <c:y val="0.101061915046796"/>
+          <c:w val="0.900445389209434"/>
+          <c:h val="0.746625269978402"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -905,11 +940,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="63716207"/>
-        <c:axId val="16977"/>
+        <c:axId val="48826424"/>
+        <c:axId val="41061981"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63716207"/>
+        <c:axId val="48826424"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -977,14 +1012,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16977"/>
+        <c:crossAx val="41061981"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16977"/>
+        <c:axId val="41061981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1060,7 +1095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63716207"/>
+        <c:crossAx val="48826424"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -2137,11 +2172,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49806575"/>
-        <c:axId val="55424121"/>
+        <c:axId val="90408530"/>
+        <c:axId val="17911798"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49806575"/>
+        <c:axId val="90408530"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -2208,13 +2243,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55424121"/>
+        <c:crossAx val="17911798"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55424121"/>
+        <c:axId val="17911798"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -2290,7 +2325,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49806575"/>
+        <c:crossAx val="90408530"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2354,43 +2389,46 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$82</c:f>
+              <c:f>Baseline_100pkt!$L$150</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>Board 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff6d6d"/>
+              <a:srgbClr val="f10d0c"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ff6d6d"/>
+                <a:srgbClr val="f10d0c"/>
               </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="triangle"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff6d6d"/>
+                <a:srgbClr val="f10d0c"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dPt>
             <c:idx val="0"/>
             <c:marker>
-              <c:symbol val="square"/>
+              <c:symbol val="triangle"/>
               <c:size val="8"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:srgbClr val="ff6d6d"/>
+                  <a:srgbClr val="f10d0c"/>
                 </a:solidFill>
               </c:spPr>
             </c:marker>
@@ -2481,7 +2519,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="ff6d6d"/>
+                  <a:srgbClr val="f10d0c"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2529,23 +2567,26 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$86</c:f>
+              <c:f>Baseline_100pkt!$L$151</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>Board 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="f10d0c"/>
+              <a:srgbClr val="3465a4"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="f10d0c"/>
+                <a:srgbClr val="3465a4"/>
               </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -2554,7 +2595,7 @@
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="f10d0c"/>
+                <a:srgbClr val="3465a4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -2623,7 +2664,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="f10d0c"/>
+                  <a:srgbClr val="3465a4"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2671,23 +2712,26 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$90</c:f>
+              <c:f>Baseline_100pkt!$L$152</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>Board 3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="ff3838"/>
+              <a:srgbClr val="069a2e"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ff3838"/>
+                <a:srgbClr val="069a2e"/>
               </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -2696,44 +2740,11 @@
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ff3838"/>
+                <a:srgbClr val="069a2e"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="triangle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="ff3838"/>
-                </a:solidFill>
-              </c:spPr>
-            </c:marker>
-          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -2798,7 +2809,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="ff3838"/>
+                  <a:srgbClr val="069a2e"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2846,32 +2857,32 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$95</c:f>
+              <c:f>Baseline_100pkt!$L$153</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 MAC</c:v>
+                  <c:v>Board 1 MAC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="069a2e"/>
+              <a:srgbClr val="f10d0c"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="069a2e"/>
+                <a:srgbClr val="f10d0c"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
+            <c:symbol val="triangle"/>
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="069a2e"/>
+                <a:srgbClr val="f10d0c"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -2940,7 +2951,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="069a2e"/>
+                  <a:srgbClr val="f10d0c"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -2988,22 +2999,22 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$99</c:f>
+              <c:f>Baseline_100pkt!$L$154</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2 MAC</c:v>
+                  <c:v>Board 2 MAC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="3faf46"/>
+              <a:srgbClr val="3465a4"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="3faf46"/>
+                <a:srgbClr val="3465a4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3013,7 +3024,7 @@
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="3faf46"/>
+                <a:srgbClr val="3465a4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -3082,7 +3093,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="3faf46"/>
+                  <a:srgbClr val="3465a4"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -3130,22 +3141,22 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$N$103</c:f>
+              <c:f>Baseline_100pkt!$L$155</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3 MAC</c:v>
+                  <c:v>Board 3 MAC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="77bc65"/>
+              <a:srgbClr val="069a2e"/>
             </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="77bc65"/>
+                <a:srgbClr val="069a2e"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3155,7 +3166,7 @@
             <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="77bc65"/>
+                <a:srgbClr val="069a2e"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
@@ -3166,7 +3177,7 @@
               <c:size val="8"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:srgbClr val="77bc65"/>
+                  <a:srgbClr val="069a2e"/>
                 </a:solidFill>
               </c:spPr>
             </c:marker>
@@ -3257,7 +3268,7 @@
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="77bc65"/>
+                  <a:srgbClr val="069a2e"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
@@ -3300,11 +3311,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15831808"/>
-        <c:axId val="90436232"/>
+        <c:axId val="97316583"/>
+        <c:axId val="87434652"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15831808"/>
+        <c:axId val="97316583"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -3371,13 +3382,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90436232"/>
+        <c:crossAx val="87434652"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90436232"/>
+        <c:axId val="87434652"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3453,7 +3464,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15831808"/>
+        <c:crossAx val="97316583"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -3514,10 +3525,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501290551141252"/>
-          <c:y val="0.101048274620957"/>
-          <c:w val="0.900526342426236"/>
-          <c:h val="0.746659468214334"/>
+          <c:x val="0.0501315922664237"/>
+          <c:y val="0.101061915046796"/>
+          <c:w val="0.900445389209434"/>
+          <c:h val="0.746625269978402"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3807,11 +3818,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="47505677"/>
-        <c:axId val="31888316"/>
+        <c:axId val="4743745"/>
+        <c:axId val="48770177"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47505677"/>
+        <c:axId val="4743745"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -3879,14 +3890,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31888316"/>
+        <c:crossAx val="48770177"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31888316"/>
+        <c:axId val="48770177"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3962,7 +3973,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47505677"/>
+        <c:crossAx val="4743745"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -4012,20 +4023,354 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$AD$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no fault</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="a7074b"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$AE$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.7434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$AD$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fault</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="168253"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$AE$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.4157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$AD$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>redundant</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3465a4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$AE$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.8427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="72453050"/>
+        <c:axId val="7696785"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="72453050"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7696785"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7696785"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>package delivery ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="72453050"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>486720</xdr:colOff>
+      <xdr:colOff>487080</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>99360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>287640</xdr:colOff>
+      <xdr:colOff>286920</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>214200</xdr:rowOff>
+      <xdr:rowOff>213120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4033,8 +4378,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33294600" y="16205400"/>
-        <a:ext cx="14226120" cy="8001360"/>
+        <a:off x="33295320" y="16205400"/>
+        <a:ext cx="14225400" cy="8000280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4047,15 +4392,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
+      <xdr:colOff>777600</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1873800</xdr:colOff>
+      <xdr:colOff>1873080</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>36720</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4063,8 +4408,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17734680" y="25659360"/>
-        <a:ext cx="14335200" cy="8062560"/>
+        <a:off x="17735040" y="25659720"/>
+        <a:ext cx="14334480" cy="8061480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4077,15 +4422,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>794160</xdr:colOff>
+      <xdr:colOff>794520</xdr:colOff>
       <xdr:row>149</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1890720</xdr:colOff>
+      <xdr:colOff>1890000</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>116640</xdr:rowOff>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4093,8 +4438,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17751600" y="34045200"/>
-        <a:ext cx="14335200" cy="8021880"/>
+        <a:off x="17751960" y="34045560"/>
+        <a:ext cx="14334480" cy="8020800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4107,15 +4452,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>2609280</xdr:colOff>
+      <xdr:colOff>2609640</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>611280</xdr:colOff>
+      <xdr:colOff>610560</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4123,12 +4468,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="32805360" y="24498000"/>
-        <a:ext cx="14226120" cy="8001360"/>
+        <a:off x="32806080" y="24498360"/>
+        <a:ext cx="14225400" cy="8000280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>29160</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>118080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>511200</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>52200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="48075480" y="14722920"/>
+        <a:ext cx="7783560" cy="4377960"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4144,11 +4519,11 @@
   </sheetPr>
   <dimension ref="A1:AP182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P96" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U170" activeCellId="0" sqref="U170"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W35" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH70" activeCellId="0" sqref="AH70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
@@ -4173,8 +4548,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="25.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="32.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="33.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="30.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="34.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="33.74"/>
@@ -8546,6 +8921,12 @@
       <c r="Y57" s="14" t="s">
         <v>32</v>
       </c>
+      <c r="AD57" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE57" s="16" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
@@ -8559,10 +8940,10 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="O58" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="P58" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q58" s="17" t="n">
         <f aca="false">I49</f>
@@ -8579,10 +8960,10 @@
         <v>30</v>
       </c>
       <c r="U58" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="V58" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="W58" s="17" t="n">
         <f aca="false">I75</f>
@@ -8595,6 +8976,12 @@
       <c r="Y58" s="17" t="n">
         <f aca="false">STDEV(W58:W60)</f>
         <v>0.013471506281091</v>
+      </c>
+      <c r="AD58" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE58" s="16" t="n">
+        <v>0.7434</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8635,7 +9022,7 @@
       <c r="M59" s="7"/>
       <c r="O59" s="14"/>
       <c r="P59" s="16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q59" s="17" t="n">
         <f aca="false">I50</f>
@@ -8646,7 +9033,7 @@
       <c r="T59" s="16"/>
       <c r="U59" s="14"/>
       <c r="V59" s="16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="W59" s="17" t="n">
         <f aca="false">I76</f>
@@ -8654,6 +9041,12 @@
       </c>
       <c r="X59" s="17"/>
       <c r="Y59" s="17"/>
+      <c r="AD59" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE59" s="16" t="n">
+        <v>0.4157</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
@@ -8695,7 +9088,7 @@
       <c r="M60" s="7"/>
       <c r="O60" s="14"/>
       <c r="P60" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="Q60" s="17" t="n">
         <f aca="false">I51</f>
@@ -8706,7 +9099,7 @@
       <c r="T60" s="16"/>
       <c r="U60" s="14"/>
       <c r="V60" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="W60" s="17" t="n">
         <f aca="false">I77</f>
@@ -8714,6 +9107,12 @@
       </c>
       <c r="X60" s="17"/>
       <c r="Y60" s="17"/>
+      <c r="AD60" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE60" s="16" t="n">
+        <v>0.8427</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
@@ -8754,10 +9153,10 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
       <c r="O61" s="14" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="P61" s="16" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="Q61" s="17" t="n">
         <f aca="false">X23</f>
@@ -8774,10 +9173,10 @@
         <v>15</v>
       </c>
       <c r="U61" s="14" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="V61" s="16" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="W61" s="17" t="n">
         <f aca="false">X49</f>
@@ -8832,7 +9231,7 @@
       <c r="M62" s="7"/>
       <c r="O62" s="14"/>
       <c r="P62" s="16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="Q62" s="17" t="n">
         <f aca="false">X24</f>
@@ -8843,7 +9242,7 @@
       <c r="T62" s="16"/>
       <c r="U62" s="14"/>
       <c r="V62" s="16" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W62" s="17" t="n">
         <f aca="false">X50</f>
@@ -8865,7 +9264,7 @@
       <c r="M63" s="4"/>
       <c r="O63" s="14"/>
       <c r="P63" s="16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Q63" s="17" t="n">
         <f aca="false">X25</f>
@@ -8876,7 +9275,7 @@
       <c r="T63" s="16"/>
       <c r="U63" s="14"/>
       <c r="V63" s="16" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="W63" s="17" t="n">
         <f aca="false">X51</f>
@@ -8922,10 +9321,10 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
       <c r="O64" s="14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="P64" s="16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Q64" s="17" t="n">
         <f aca="false">AL23</f>
@@ -8942,10 +9341,10 @@
         <v>5</v>
       </c>
       <c r="U64" s="14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="V64" s="16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="W64" s="17" t="n">
         <f aca="false">AL49</f>
@@ -9000,7 +9399,7 @@
       <c r="M65" s="7"/>
       <c r="O65" s="14"/>
       <c r="P65" s="16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Q65" s="17" t="n">
         <f aca="false">AL24</f>
@@ -9011,7 +9410,7 @@
       <c r="T65" s="16"/>
       <c r="U65" s="14"/>
       <c r="V65" s="16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="W65" s="17" t="n">
         <f aca="false">AL50</f>
@@ -9060,7 +9459,7 @@
       <c r="M66" s="7"/>
       <c r="O66" s="14"/>
       <c r="P66" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="Q66" s="17" t="n">
         <f aca="false">AL25</f>
@@ -9071,7 +9470,7 @@
       <c r="T66" s="16"/>
       <c r="U66" s="14"/>
       <c r="V66" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="W66" s="17" t="n">
         <f aca="false">AL51</f>
@@ -9123,22 +9522,22 @@
       <c r="A68" s="4"/>
       <c r="D68" s="4"/>
       <c r="O68" s="16" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="P68" s="16" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="Q68" s="16" t="s">
         <v>33</v>
       </c>
       <c r="R68" s="16" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S68" s="16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="T68" s="16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9360,7 +9759,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="O73" s="18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="P73" s="17" t="n">
         <f aca="false">X58</f>
@@ -9600,7 +9999,7 @@
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
       <c r="O77" s="16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="P77" s="20"/>
       <c r="Q77" s="19"/>
@@ -9613,7 +10012,7 @@
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O78" s="16" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P78" s="20"/>
       <c r="Q78" s="19"/>
@@ -9628,16 +10027,16 @@
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="81" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N81" s="16" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P81" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Q81" s="16" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R81" s="16" t="s">
         <v>33</v>
@@ -9648,7 +10047,7 @@
         <v>1</v>
       </c>
       <c r="O82" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P82" s="17" t="n">
         <f aca="false">Q58</f>
@@ -9665,7 +10064,7 @@
     <row r="83" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N83" s="16"/>
       <c r="O83" s="16" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="P83" s="17" t="n">
         <f aca="false">Q61</f>
@@ -9682,7 +10081,7 @@
     <row r="84" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N84" s="16"/>
       <c r="O84" s="16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="P84" s="17" t="n">
         <f aca="false">Q64</f>
@@ -9708,7 +10107,7 @@
         <v>2</v>
       </c>
       <c r="O86" s="16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="P86" s="17" t="n">
         <f aca="false">Q59</f>
@@ -9725,7 +10124,7 @@
     <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N87" s="16"/>
       <c r="O87" s="16" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="P87" s="17" t="n">
         <f aca="false">Q62</f>
@@ -9742,7 +10141,7 @@
     <row r="88" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N88" s="16"/>
       <c r="O88" s="16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P88" s="17" t="n">
         <f aca="false">Q65</f>
@@ -9768,7 +10167,7 @@
         <v>3</v>
       </c>
       <c r="O90" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="P90" s="17" t="n">
         <f aca="false">Q60</f>
@@ -9785,7 +10184,7 @@
     <row r="91" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N91" s="16"/>
       <c r="O91" s="16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="P91" s="17" t="n">
         <f aca="false">Q63</f>
@@ -9802,7 +10201,7 @@
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N92" s="16"/>
       <c r="O92" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="P92" s="17" t="n">
         <f aca="false">Q66</f>
@@ -9832,10 +10231,10 @@
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N95" s="16" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="O95" s="16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P95" s="17" t="n">
         <f aca="false">W58</f>
@@ -9852,7 +10251,7 @@
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N96" s="16"/>
       <c r="O96" s="16" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="P96" s="17" t="n">
         <f aca="false">W61</f>
@@ -9869,7 +10268,7 @@
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N97" s="16"/>
       <c r="O97" s="16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="P97" s="17" t="n">
         <f aca="false">W64</f>
@@ -9892,10 +10291,10 @@
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N99" s="16" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="O99" s="16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="P99" s="17" t="n">
         <f aca="false">W59</f>
@@ -9912,7 +10311,7 @@
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N100" s="16"/>
       <c r="O100" s="16" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P100" s="17" t="n">
         <f aca="false">W62</f>
@@ -9929,7 +10328,7 @@
     <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N101" s="16"/>
       <c r="O101" s="16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="P101" s="17" t="n">
         <f aca="false">W65</f>
@@ -9952,10 +10351,10 @@
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N103" s="16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="O103" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P103" s="17" t="n">
         <f aca="false">W60</f>
@@ -9972,7 +10371,7 @@
     <row r="104" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N104" s="16"/>
       <c r="O104" s="16" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P104" s="17" t="n">
         <f aca="false">W63</f>
@@ -9989,7 +10388,7 @@
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N105" s="16"/>
       <c r="O105" s="16" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="P105" s="17" t="n">
         <f aca="false">W66</f>
@@ -10047,12 +10446,36 @@
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L150" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L151" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L152" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L153" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L154" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L155" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10170,7 +10593,7 @@
   </sheetPr>
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -10193,7 +10616,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -10267,10 +10690,10 @@
         <v>0.96</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>-101.07</v>
@@ -10293,10 +10716,10 @@
         <v>0.96</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>-101.22</v>
@@ -10319,10 +10742,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>-101.29</v>
@@ -10373,10 +10796,10 @@
         <v>0.88</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G15" s="9" t="n">
         <v>-101.17</v>
@@ -10399,10 +10822,10 @@
         <v>0.96</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>-101.96</v>
@@ -10425,10 +10848,10 @@
         <v>0.96</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>-100.88</v>
@@ -10479,10 +10902,10 @@
         <v>0.93</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>-102.88</v>
@@ -10505,10 +10928,10 @@
         <v>0.96</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G21" s="9" t="n">
         <v>-103.92</v>
@@ -10531,10 +10954,10 @@
         <v>1</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>-102.07</v>
@@ -10669,12 +11092,12 @@
     </row>
     <row r="30" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -10748,10 +11171,10 @@
         <v>0.81</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G38" s="9" t="n">
         <v>-103.42</v>
@@ -10774,10 +11197,10 @@
         <v>0.81</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G39" s="9" t="n">
         <v>-102.75</v>
@@ -10800,10 +11223,10 @@
         <v>0.8</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G40" s="9" t="n">
         <v>-99.47</v>
@@ -10854,10 +11277,10 @@
         <v>0.81</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>-98.86</v>
@@ -10880,10 +11303,10 @@
         <v>0.77</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G44" s="9" t="n">
         <v>-99.63</v>
@@ -10906,10 +11329,10 @@
         <v>0.88</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G45" s="9" t="n">
         <v>-101.64</v>
@@ -10972,10 +11395,10 @@
         <v>0.92</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G48" s="9" t="n">
         <v>-89.75</v>
@@ -10998,10 +11421,10 @@
         <v>0.82</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>-102.47</v>
@@ -11024,10 +11447,10 @@
         <v>0.85</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G50" s="9" t="n">
         <v>-102.7</v>
@@ -11192,11 +11615,11 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
@@ -11214,7 +11637,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -11814,12 +12237,12 @@
     </row>
     <row r="29" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>

</xml_diff>

<commit_message>
added newest vis for data
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="88">
   <si>
     <t xml:space="preserve">Baseline 1</t>
   </si>
@@ -135,6 +135,9 @@
     <t xml:space="preserve">Redundancy experiment PDRs</t>
   </si>
   <si>
+    <t xml:space="preserve">pkt tx</t>
+  </si>
+  <si>
     <t xml:space="preserve">30s Raw LoRa</t>
   </si>
   <si>
@@ -231,6 +234,9 @@
     <t xml:space="preserve">perfomance increase sigma</t>
   </si>
   <si>
+    <t xml:space="preserve">Baseline</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAC Layer</t>
   </si>
   <si>
@@ -252,13 +258,13 @@
     <t xml:space="preserve">3 MAC</t>
   </si>
   <si>
-    <t xml:space="preserve">Board 1</t>
+    <t xml:space="preserve">Board 1 Baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">Board 2</t>
+    <t xml:space="preserve">Board 2 Baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">Board 3</t>
+    <t xml:space="preserve">Board 3 Baseline</t>
   </si>
   <si>
     <t xml:space="preserve">Board 1 MAC</t>
@@ -562,7 +568,7 @@
       <rgbColor rgb="FF127622"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FFA7074B"/>
+      <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF168253"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
@@ -593,7 +599,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF77BC65"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF3465A4"/>
@@ -611,7 +617,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -623,10 +629,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501315922664237"/>
-          <c:y val="0.101061915046796"/>
-          <c:w val="0.900445389209434"/>
-          <c:h val="0.746625269978402"/>
+          <c:x val="0.050134129675558"/>
+          <c:y val="0.101071010710107"/>
+          <c:w val="0.900389735283697"/>
+          <c:h val="0.74660246602466"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -641,7 +647,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Raw LoRa</c:v>
+                  <c:v>Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -940,11 +946,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48826424"/>
-        <c:axId val="41061981"/>
+        <c:axId val="79200103"/>
+        <c:axId val="63089363"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48826424"/>
+        <c:axId val="79200103"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -1012,14 +1018,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41061981"/>
+        <c:crossAx val="63089363"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41061981"/>
+        <c:axId val="63089363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1095,7 +1101,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48826424"/>
+        <c:crossAx val="79200103"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -1145,7 +1151,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2172,11 +2178,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="90408530"/>
-        <c:axId val="17911798"/>
+        <c:axId val="82928897"/>
+        <c:axId val="9932941"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90408530"/>
+        <c:axId val="82928897"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -2243,13 +2249,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17911798"/>
+        <c:crossAx val="9932941"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="17911798"/>
+        <c:axId val="9932941"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1"/>
@@ -2325,7 +2331,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90408530"/>
+        <c:crossAx val="82928897"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -2374,7 +2380,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2393,7 +2399,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Board 1</c:v>
+                  <c:v>Board 1 Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2571,7 +2577,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Board 2</c:v>
+                  <c:v>Board 2 Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2716,7 +2722,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Board 3</c:v>
+                  <c:v>Board 3 Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3311,11 +3317,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97316583"/>
-        <c:axId val="87434652"/>
+        <c:axId val="8011207"/>
+        <c:axId val="83109481"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97316583"/>
+        <c:axId val="8011207"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -3382,13 +3388,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87434652"/>
+        <c:crossAx val="83109481"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87434652"/>
+        <c:axId val="83109481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3464,7 +3470,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97316583"/>
+        <c:crossAx val="8011207"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -3513,7 +3519,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3525,10 +3531,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0501315922664237"/>
-          <c:y val="0.101061915046796"/>
-          <c:w val="0.900445389209434"/>
-          <c:h val="0.746625269978402"/>
+          <c:x val="0.050134129675558"/>
+          <c:y val="0.101071010710107"/>
+          <c:w val="0.900389735283697"/>
+          <c:h val="0.74660246602466"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3543,7 +3549,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Raw LoRa</c:v>
+                  <c:v>Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3818,11 +3824,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4743745"/>
-        <c:axId val="48770177"/>
+        <c:axId val="11905682"/>
+        <c:axId val="98694400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4743745"/>
+        <c:axId val="11905682"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="35"/>
@@ -3890,14 +3896,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48770177"/>
+        <c:crossAx val="98694400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48770177"/>
+        <c:axId val="98694400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3973,7 +3979,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4743745"/>
+        <c:crossAx val="11905682"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
@@ -4023,7 +4029,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4039,67 +4045,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$AD$58</c:f>
+              <c:f>Baseline_100pkt!$AD$58:$AD$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>no fault</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="a7074b"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Baseline_100pkt!$AE$58</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.7434</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Baseline_100pkt!$AD$59</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>fault</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4125,6 +4075,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4135,12 +4086,69 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Baseline_100pkt!$AE$59</c:f>
+              <c:f>Baseline_100pkt!$AE$58:$AE$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.4157</c:v>
+                  <c:v>0.7434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$AD$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>no fault</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$AE$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.7434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4151,11 +4159,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Baseline_100pkt!$AD$60</c:f>
+              <c:f>Baseline_100pkt!$AD$59:$AD$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>redundant</c:v>
+                  <c:v>fault</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4181,6 +4189,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4191,12 +4200,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Baseline_100pkt!$AE$60</c:f>
+              <c:f>Baseline_100pkt!$AE$59:$AE$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.8427</c:v>
+                  <c:v>0.4157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4204,11 +4213,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="72453050"/>
-        <c:axId val="7696785"/>
+        <c:axId val="83241949"/>
+        <c:axId val="11274034"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72453050"/>
+        <c:axId val="83241949"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4236,7 +4245,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7696785"/>
+        <c:crossAx val="11274034"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4244,7 +4253,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7696785"/>
+        <c:axId val="11274034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4287,7 +4296,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4309,7 +4318,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72453050"/>
+        <c:crossAx val="83241949"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4350,7 +4359,1362 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$150</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 1 Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="f10d0c"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$82:$R$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$82:$P$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.863333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.623333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$151</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 2 Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3465a4"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="3465a4"/>
+              </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3465a4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$86:$R$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$86:$P$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.486666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.616666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.436666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$152</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 3 Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+              <a:custDash>
+                <a:ds d="197000" sp="127000"/>
+              </a:custDash>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$90:$R$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$90:$P$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.676666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.556666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$153</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 1 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$95:$R$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$95:$P$97</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.916666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.616666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$154</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 2 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3465a4"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="3465a4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3465a4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$99:$R$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$99:$P$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.966666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.523333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$L$155</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Board 3 MAC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="069a2e"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$R$103:$R$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$103:$P$105</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.946666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.966666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="66796444"/>
+        <c:axId val="42642176"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="66796444"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="35"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Transmission interval (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42642176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="42642176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1600" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Packet delivery ratio (PDR)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="66796444"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1600" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.050134129675558"/>
+          <c:y val="0.101071010710107"/>
+          <c:w val="0.900389735283697"/>
+          <c:h val="0.74660246602466"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$O$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Baseline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="f10d0c"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="f10d0c"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.117015351952607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.130398250385899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0945946517946345</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$69:$R$71</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.117015351952607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.130398250385899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0945946517946345</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="f10d0c"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$Q$69:$Q$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$69:$P$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Baseline_100pkt!$O$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MAC Layer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="069a2e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="069a2e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.013471506281091</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0835330939076111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Baseline_100pkt!$R$73:$R$75</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.013471506281091</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0288675134594813</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0835330939076111</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="069a2e"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$Q$73:$Q$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Baseline_100pkt!$P$73:$P$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.962222222222222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="15847496"/>
+        <c:axId val="3323568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="15847496"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+          <c:max val="35"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Transmission interval (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12600">
+            <a:solidFill>
+              <a:srgbClr val="cccccc"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="3323568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="3323568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="dddddd"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Packet delivery ratio (PDR)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="15847496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.05"/>
+        <c:minorUnit val="0.025"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -4368,9 +5732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>286920</xdr:colOff>
+      <xdr:colOff>286200</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>213120</xdr:rowOff>
+      <xdr:rowOff>212400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4379,7 +5743,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="33295320" y="16205400"/>
-        <a:ext cx="14225400" cy="8000280"/>
+        <a:ext cx="14224680" cy="7999560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4398,9 +5762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1873080</xdr:colOff>
+      <xdr:colOff>1872360</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4409,7 +5773,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17735040" y="25659720"/>
-        <a:ext cx="14334480" cy="8061480"/>
+        <a:ext cx="14333760" cy="8060760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4428,9 +5792,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1890000</xdr:colOff>
+      <xdr:colOff>1889280</xdr:colOff>
       <xdr:row>193</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4439,7 +5803,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="17751960" y="34045560"/>
-        <a:ext cx="14334480" cy="8020800"/>
+        <a:ext cx="14333760" cy="8020080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4458,9 +5822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>610560</xdr:colOff>
+      <xdr:colOff>609840</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>146160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4469,7 +5833,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="32806080" y="24498360"/>
-        <a:ext cx="14225400" cy="8000280"/>
+        <a:ext cx="14224680" cy="7999560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4488,9 +5852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>511200</xdr:colOff>
+      <xdr:colOff>510480</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>52200</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4499,11 +5863,71 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="48075480" y="14722920"/>
-        <a:ext cx="7783560" cy="4377960"/>
+        <a:ext cx="7781400" cy="4377240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>2592000</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>177840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>701280</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>151200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="32788440" y="34244280"/>
+        <a:ext cx="14333760" cy="8020080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>33120</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>126720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>141480</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="48079440" y="24369480"/>
+        <a:ext cx="16838280" cy="9131400"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4519,11 +5943,11 @@
   </sheetPr>
   <dimension ref="A1:AP182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W35" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH70" activeCellId="0" sqref="AH70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V116" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T164" activeCellId="0" sqref="T164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.29"/>
@@ -4548,7 +5972,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="25.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="32.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="30.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="30.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="34.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="13.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.89"/>
@@ -8927,6 +10351,9 @@
       <c r="AE57" s="16" t="s">
         <v>36</v>
       </c>
+      <c r="AF57" s="16" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
@@ -8940,10 +10367,10 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="O58" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P58" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q58" s="17" t="n">
         <f aca="false">I49</f>
@@ -8960,10 +10387,10 @@
         <v>30</v>
       </c>
       <c r="U58" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V58" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W58" s="17" t="n">
         <f aca="false">I75</f>
@@ -8978,11 +10405,12 @@
         <v>0.013471506281091</v>
       </c>
       <c r="AD58" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AE58" s="16" t="n">
         <v>0.7434</v>
       </c>
+      <c r="AF58" s="16"/>
     </row>
     <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
@@ -9022,7 +10450,7 @@
       <c r="M59" s="7"/>
       <c r="O59" s="14"/>
       <c r="P59" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q59" s="17" t="n">
         <f aca="false">I50</f>
@@ -9033,7 +10461,7 @@
       <c r="T59" s="16"/>
       <c r="U59" s="14"/>
       <c r="V59" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="W59" s="17" t="n">
         <f aca="false">I76</f>
@@ -9042,10 +10470,13 @@
       <c r="X59" s="17"/>
       <c r="Y59" s="17"/>
       <c r="AD59" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AE59" s="16" t="n">
         <v>0.4157</v>
+      </c>
+      <c r="AF59" s="16" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9088,7 +10519,7 @@
       <c r="M60" s="7"/>
       <c r="O60" s="14"/>
       <c r="P60" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q60" s="17" t="n">
         <f aca="false">I51</f>
@@ -9099,7 +10530,7 @@
       <c r="T60" s="16"/>
       <c r="U60" s="14"/>
       <c r="V60" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W60" s="17" t="n">
         <f aca="false">I77</f>
@@ -9108,10 +10539,13 @@
       <c r="X60" s="17"/>
       <c r="Y60" s="17"/>
       <c r="AD60" s="16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AE60" s="16" t="n">
         <v>0.8427</v>
+      </c>
+      <c r="AF60" s="16" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9153,10 +10587,10 @@
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
       <c r="O61" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P61" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q61" s="17" t="n">
         <f aca="false">X23</f>
@@ -9173,10 +10607,10 @@
         <v>15</v>
       </c>
       <c r="U61" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="V61" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="W61" s="17" t="n">
         <f aca="false">X49</f>
@@ -9231,7 +10665,7 @@
       <c r="M62" s="7"/>
       <c r="O62" s="14"/>
       <c r="P62" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q62" s="17" t="n">
         <f aca="false">X24</f>
@@ -9242,7 +10676,7 @@
       <c r="T62" s="16"/>
       <c r="U62" s="14"/>
       <c r="V62" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W62" s="17" t="n">
         <f aca="false">X50</f>
@@ -9264,7 +10698,7 @@
       <c r="M63" s="4"/>
       <c r="O63" s="14"/>
       <c r="P63" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q63" s="17" t="n">
         <f aca="false">X25</f>
@@ -9275,7 +10709,7 @@
       <c r="T63" s="16"/>
       <c r="U63" s="14"/>
       <c r="V63" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W63" s="17" t="n">
         <f aca="false">X51</f>
@@ -9321,10 +10755,10 @@
       <c r="L64" s="7"/>
       <c r="M64" s="7"/>
       <c r="O64" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P64" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q64" s="17" t="n">
         <f aca="false">AL23</f>
@@ -9341,10 +10775,10 @@
         <v>5</v>
       </c>
       <c r="U64" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V64" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W64" s="17" t="n">
         <f aca="false">AL49</f>
@@ -9399,7 +10833,7 @@
       <c r="M65" s="7"/>
       <c r="O65" s="14"/>
       <c r="P65" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q65" s="17" t="n">
         <f aca="false">AL24</f>
@@ -9410,7 +10844,7 @@
       <c r="T65" s="16"/>
       <c r="U65" s="14"/>
       <c r="V65" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W65" s="17" t="n">
         <f aca="false">AL50</f>
@@ -9459,7 +10893,7 @@
       <c r="M66" s="7"/>
       <c r="O66" s="14"/>
       <c r="P66" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q66" s="17" t="n">
         <f aca="false">AL25</f>
@@ -9470,7 +10904,7 @@
       <c r="T66" s="16"/>
       <c r="U66" s="14"/>
       <c r="V66" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="W66" s="17" t="n">
         <f aca="false">AL51</f>
@@ -9522,22 +10956,22 @@
       <c r="A68" s="4"/>
       <c r="D68" s="4"/>
       <c r="O68" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P68" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q68" s="16" t="s">
         <v>33</v>
       </c>
       <c r="R68" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S68" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T68" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9577,7 +11011,7 @@
       <c r="L69" s="7"/>
       <c r="M69" s="7"/>
       <c r="O69" s="18" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="P69" s="17" t="n">
         <f aca="false">R58</f>
@@ -9759,7 +11193,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="O73" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P73" s="17" t="n">
         <f aca="false">X58</f>
@@ -9999,7 +11433,7 @@
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
       <c r="O77" s="16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P77" s="20"/>
       <c r="Q77" s="19"/>
@@ -10012,7 +11446,7 @@
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O78" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P78" s="20"/>
       <c r="Q78" s="19"/>
@@ -10030,13 +11464,13 @@
         <v>35</v>
       </c>
       <c r="O81" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="P81" s="16" t="s">
         <v>12</v>
       </c>
       <c r="Q81" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R81" s="16" t="s">
         <v>33</v>
@@ -10047,7 +11481,7 @@
         <v>1</v>
       </c>
       <c r="O82" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P82" s="17" t="n">
         <f aca="false">Q58</f>
@@ -10064,7 +11498,7 @@
     <row r="83" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N83" s="16"/>
       <c r="O83" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P83" s="17" t="n">
         <f aca="false">Q61</f>
@@ -10081,7 +11515,7 @@
     <row r="84" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N84" s="16"/>
       <c r="O84" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P84" s="17" t="n">
         <f aca="false">Q64</f>
@@ -10107,7 +11541,7 @@
         <v>2</v>
       </c>
       <c r="O86" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P86" s="17" t="n">
         <f aca="false">Q59</f>
@@ -10124,7 +11558,7 @@
     <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N87" s="16"/>
       <c r="O87" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P87" s="17" t="n">
         <f aca="false">Q62</f>
@@ -10141,7 +11575,7 @@
     <row r="88" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N88" s="16"/>
       <c r="O88" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P88" s="17" t="n">
         <f aca="false">Q65</f>
@@ -10167,7 +11601,7 @@
         <v>3</v>
       </c>
       <c r="O90" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P90" s="17" t="n">
         <f aca="false">Q60</f>
@@ -10184,7 +11618,7 @@
     <row r="91" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N91" s="16"/>
       <c r="O91" s="16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="P91" s="17" t="n">
         <f aca="false">Q63</f>
@@ -10201,7 +11635,7 @@
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N92" s="16"/>
       <c r="O92" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P92" s="17" t="n">
         <f aca="false">Q66</f>
@@ -10231,10 +11665,10 @@
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N95" s="16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O95" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P95" s="17" t="n">
         <f aca="false">W58</f>
@@ -10251,7 +11685,7 @@
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N96" s="16"/>
       <c r="O96" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P96" s="17" t="n">
         <f aca="false">W61</f>
@@ -10268,7 +11702,7 @@
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N97" s="16"/>
       <c r="O97" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P97" s="17" t="n">
         <f aca="false">W64</f>
@@ -10291,10 +11725,10 @@
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N99" s="16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O99" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="P99" s="17" t="n">
         <f aca="false">W59</f>
@@ -10311,7 +11745,7 @@
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N100" s="16"/>
       <c r="O100" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P100" s="17" t="n">
         <f aca="false">W62</f>
@@ -10328,7 +11762,7 @@
     <row r="101" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N101" s="16"/>
       <c r="O101" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P101" s="17" t="n">
         <f aca="false">W65</f>
@@ -10351,10 +11785,10 @@
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N103" s="16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O103" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P103" s="17" t="n">
         <f aca="false">W60</f>
@@ -10371,7 +11805,7 @@
     <row r="104" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N104" s="16"/>
       <c r="O104" s="16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P104" s="17" t="n">
         <f aca="false">W63</f>
@@ -10388,7 +11822,7 @@
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N105" s="16"/>
       <c r="O105" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P105" s="17" t="n">
         <f aca="false">W66</f>
@@ -10448,32 +11882,32 @@
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L150" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L151" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L152" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L153" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L154" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L155" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10593,7 +12027,7 @@
   </sheetPr>
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -10616,7 +12050,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -10690,10 +12124,10 @@
         <v>0.96</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>-101.07</v>
@@ -10716,10 +12150,10 @@
         <v>0.96</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G11" s="9" t="n">
         <v>-101.22</v>
@@ -10742,10 +12176,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G12" s="9" t="n">
         <v>-101.29</v>
@@ -10796,10 +12230,10 @@
         <v>0.88</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G15" s="9" t="n">
         <v>-101.17</v>
@@ -10822,10 +12256,10 @@
         <v>0.96</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G16" s="9" t="n">
         <v>-101.96</v>
@@ -10848,10 +12282,10 @@
         <v>0.96</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G17" s="9" t="n">
         <v>-100.88</v>
@@ -10902,10 +12336,10 @@
         <v>0.93</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G20" s="9" t="n">
         <v>-102.88</v>
@@ -10928,10 +12362,10 @@
         <v>0.96</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G21" s="9" t="n">
         <v>-103.92</v>
@@ -10954,10 +12388,10 @@
         <v>1</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G22" s="9" t="n">
         <v>-102.07</v>
@@ -11092,12 +12526,12 @@
     </row>
     <row r="30" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -11171,10 +12605,10 @@
         <v>0.81</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G38" s="9" t="n">
         <v>-103.42</v>
@@ -11197,10 +12631,10 @@
         <v>0.81</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G39" s="9" t="n">
         <v>-102.75</v>
@@ -11223,10 +12657,10 @@
         <v>0.8</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G40" s="9" t="n">
         <v>-99.47</v>
@@ -11277,10 +12711,10 @@
         <v>0.81</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G43" s="9" t="n">
         <v>-98.86</v>
@@ -11303,10 +12737,10 @@
         <v>0.77</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G44" s="9" t="n">
         <v>-99.63</v>
@@ -11329,10 +12763,10 @@
         <v>0.88</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G45" s="9" t="n">
         <v>-101.64</v>
@@ -11395,10 +12829,10 @@
         <v>0.92</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G48" s="9" t="n">
         <v>-89.75</v>
@@ -11421,10 +12855,10 @@
         <v>0.82</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G49" s="9" t="n">
         <v>-102.47</v>
@@ -11447,10 +12881,10 @@
         <v>0.85</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G50" s="9" t="n">
         <v>-102.7</v>
@@ -11615,11 +13049,11 @@
   </sheetPr>
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.3203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
@@ -11637,7 +13071,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -12237,12 +13671,12 @@
     </row>
     <row r="29" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>

</xml_diff>